<commit_message>
numfloors jupyter notebook - include outliers query
</commit_message>
<xml_diff>
--- a/numfloors 2019-11/output/High NumFloors.xlsx
+++ b/numfloors 2019-11/output/High NumFloors.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\DCP\db-pluto-research\numfloors 2019-11\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1CE38F73-C0AB-4E54-A16F-1482DC92A3AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347E768C-257C-4E1E-8D20-0E312E4330E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Top 5 NumFloors by Boro" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="41">
   <si>
     <t>Borough</t>
   </si>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -990,12 +990,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1026,37 +1026,37 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>3067760018</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>75</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>3074357501</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>60</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>